<commit_message>
updated to hypothesis testing
</commit_message>
<xml_diff>
--- a/_Osteoporosis survey  (Responses) - Copy.xlsx
+++ b/_Osteoporosis survey  (Responses) - Copy.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9195"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
   </bookViews>
   <sheets>
     <sheet name="Form responses 1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="96">
   <si>
     <t>Timestamp</t>
   </si>
@@ -57,9 +57,6 @@
     <t>G.M bhatia</t>
   </si>
   <si>
-    <t>Calcium, Vitamin d3</t>
-  </si>
-  <si>
     <t>Teriparatide</t>
   </si>
   <si>
@@ -81,18 +78,12 @@
     <t>Uro</t>
   </si>
   <si>
-    <t>Bisphosphonate oral</t>
-  </si>
-  <si>
     <t>S.S Mohanty</t>
   </si>
   <si>
     <t xml:space="preserve">Sachin mahajan </t>
   </si>
   <si>
-    <t>Calcium, Vitamin d3, Densomab, Teriparatide</t>
-  </si>
-  <si>
     <t>Manjoo jain</t>
   </si>
   <si>
@@ -102,9 +93,6 @@
     <t>Dr atul shaa</t>
   </si>
   <si>
-    <t>Nsaids, Calcium, Vitamin d3, Bisphosphonate oral, Bisphosphonate iv</t>
-  </si>
-  <si>
     <t>Densomab</t>
   </si>
   <si>
@@ -114,60 +102,36 @@
     <t xml:space="preserve">Dr manish jain </t>
   </si>
   <si>
-    <t>Calcium, Vitamin d3, Bisphosphonate oral, Bisphosphonate iv, Teriparatide</t>
-  </si>
-  <si>
     <t xml:space="preserve">Dr M T khan </t>
   </si>
   <si>
     <t xml:space="preserve">Ramesh Wodlile </t>
   </si>
   <si>
-    <t>Nsaids, Calcium, Vitamin d3, Bisphosphonate oral, Densomab, Teriparatide</t>
-  </si>
-  <si>
     <t>Sujeet jain</t>
   </si>
   <si>
-    <t>Calcium, Vitamin d3, Teriparatide</t>
-  </si>
-  <si>
     <t>Dr namdev atam</t>
   </si>
   <si>
-    <t>Calcium, Vitamin d3, Bisphosphonate oral, Densomab, Teriparatide</t>
-  </si>
-  <si>
     <t>Jainit malviya</t>
   </si>
   <si>
     <t>Dr rajeev pathak</t>
   </si>
   <si>
-    <t>Nsaids, Calcium, Vitamin d3, Densomab, Teriparatide</t>
-  </si>
-  <si>
     <t>Keshre</t>
   </si>
   <si>
-    <t>Nsaids, Calcium, Vitamin d3, Bisphosphonate oral</t>
-  </si>
-  <si>
     <t xml:space="preserve">Dr dharish meheta </t>
   </si>
   <si>
     <t>Dr Akshay jathnkar</t>
   </si>
   <si>
-    <t>Calcium, Vitamin d3, Bisphosphonate oral, Teriparatide</t>
-  </si>
-  <si>
     <t>Hemanshu khurana</t>
   </si>
   <si>
-    <t>Nsaids, Calcium, Vitamin d3, Bisphosphonate oral, Bisphosphonate iv, Densomab, Teriparatide</t>
-  </si>
-  <si>
     <t>Sanjay popere</t>
   </si>
   <si>
@@ -183,9 +147,6 @@
     <t>Gp</t>
   </si>
   <si>
-    <t>Nsaids, Calcium, Vitamin d3</t>
-  </si>
-  <si>
     <t>Dr atul pathak</t>
   </si>
   <si>
@@ -198,39 +159,21 @@
     <t>Napro</t>
   </si>
   <si>
-    <t>Calcium, Vitamin d3, Bisphosphonate oral, Bisphosphonate iv, Densomab, Teriparatide</t>
-  </si>
-  <si>
     <t xml:space="preserve">Government hospital </t>
   </si>
   <si>
-    <t>Nsaids, Calcium, Vitamin d3, Bisphosphonate oral, Teriparatide</t>
-  </si>
-  <si>
     <t>Iravati whagmare</t>
   </si>
   <si>
-    <t>Bisphosphonate oral, Teriparatide</t>
-  </si>
-  <si>
     <t>Monika sarkate</t>
   </si>
   <si>
-    <t>Vitamin d3, Bisphosphonate oral, Bisphosphonate iv, Densomab, Teriparatide</t>
-  </si>
-  <si>
     <t>Saptdeepa das</t>
   </si>
   <si>
-    <t>Vitamin d3, Bisphosphonate iv, Densomab, Teriparatide</t>
-  </si>
-  <si>
     <t>Nirmal agarwal</t>
   </si>
   <si>
-    <t>Calcium, Vitamin d3, Bisphosphonate iv, Densomab, Teriparatide</t>
-  </si>
-  <si>
     <t>Samim aktar</t>
   </si>
   <si>
@@ -246,13 +189,1690 @@
     <t xml:space="preserve">average </t>
   </si>
   <si>
-    <t>total number</t>
-  </si>
-  <si>
-    <t>count</t>
-  </si>
-  <si>
-    <t>percentage</t>
+    <t>common therapys</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Densomab</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Teriparatide</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Densoma</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">b, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Teriparatide</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Vitamin d3, Bisphosphonate iv, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Densomab,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Teriparatide</t>
+    </r>
+  </si>
+  <si>
+    <t>teriperatide = 32</t>
+  </si>
+  <si>
+    <t>Denosamab = 25</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Calcium,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Vitamin d3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Calcium,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Vitamin d3,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Densomab</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Teriparatide</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Calcium,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Vitamin d3, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Densomab</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Teriparatide</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Calcium,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Vitamin d3, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Densomab</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Teriparatide</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Calcium,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Vitamin d3, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Densomab</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Teriparatide</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Calcium,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Vitamin d3, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Teriparatide</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Calcium,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Vitamin d3, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Densomab,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Teriparatide</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Calcium,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Vitamin d3, Bisphosphonate iv, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Densomab,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Teriparatide</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Calcium,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Vitamin d3, Bisphosphonate iv, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Densomab,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> T</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>eriparatide</t>
+    </r>
+  </si>
+  <si>
+    <t>Calcium =39</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nsaids,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Calcium,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Vitamin d3, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Densomab</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Teriparatide</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nsaids,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Calcium,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Vitamin d3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nsaids,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Calcium,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Vitamin d3, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Densomab,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Teriparatide</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Bisphosphonate </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF002060"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>oral</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nsaids,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Calcium,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Vitamin d3, Bisphosphonate </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF002060"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>oral,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Bisphosphonate iv</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Calcium,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Vitamin d3, Bisphosphonate </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF002060"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>oral,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Bisphosphonate iv, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Teriparatide</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nsaids,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Calcium,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Vitamin d3, Bisphosphonate </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF002060"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>oral,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Densomab</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Teriparatide</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Calcium,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Vitamin d3, Bisphosphonate </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF002060"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>oral,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Densomab</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Teriparatide</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nsaids,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Calcium,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Vitamin d3, Bisphosphonate </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF002060"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>oral</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Calcium,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Vitamin d3, Bisphosphonate </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF002060"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>oral,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Teriparatide</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nsaids,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Calcium,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Vitamin d3, Bisphosphonate </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF002060"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>oral,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Bisphosphonate iv, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Densomab</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Teriparatide</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nsaids,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Calcium,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Vitamin d3, Bisphosphonate </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF002060"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>oral,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Bisphosphonate iv, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Densoma</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">b, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Teriparatide</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Calcium,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Vitamin d3, Bisphosphonate </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF002060"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>oral,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Densomab</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Teriparatide</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Calcium,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Vitamin d3, Bisphosphonate </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF002060"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>oral,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Bisphosphonate iv, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Densomab</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Teriparatide</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nsaids,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Calcium,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Vitamin d3, Bisphosphonate </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF002060"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>oral,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Teriparatide</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Bisphosphonate </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF002060"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>oral,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Teriparatide</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Vitamin d3, Bisphosphonate </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF002060"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>oral,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Bisphosphonate iv, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Densomab,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Teriparatide</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Calcium,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Vitamin d3, Bisphosphonate </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF002060"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>oral,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Bisphosphonate iv, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Densomab,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Teriparatide</t>
+    </r>
+  </si>
+  <si>
+    <t>bisphosphonate oral = 17</t>
+  </si>
+  <si>
+    <t>bisphosphonate I.V = 14</t>
+  </si>
+  <si>
+    <t>vitamin d3 = 37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">do they use </t>
+  </si>
+  <si>
+    <t>denosamab = 29</t>
+  </si>
+  <si>
+    <t>terapratide = 35</t>
   </si>
 </sst>
 </file>
@@ -262,7 +1882,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -273,6 +1893,55 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFC000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF92D050"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF002060"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -296,13 +1965,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -522,11 +2194,11 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G53"/>
+  <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D57" sqref="D57"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E62" sqref="E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -537,7 +2209,7 @@
     <col min="7" max="13" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -560,7 +2232,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>45179.633985081018</v>
       </c>
@@ -573,15 +2245,15 @@
       <c r="D2" s="4">
         <v>7</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>9</v>
+      <c r="E2" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>9</v>
       </c>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>45179.634763414353</v>
       </c>
@@ -594,15 +2266,15 @@
       <c r="D3" s="4">
         <v>3</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>9</v>
+      <c r="E3" s="6" t="s">
+        <v>58</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>9</v>
       </c>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>45179.635124282402</v>
       </c>
@@ -615,20 +2287,20 @@
       <c r="D4" s="4">
         <v>4</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>13</v>
-      </c>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>45179.635413240743</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>8</v>
@@ -636,16 +2308,16 @@
       <c r="D5" s="4">
         <v>5</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E5" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>45179.635706469911</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>8</v>
@@ -653,16 +2325,16 @@
       <c r="D6" s="4">
         <v>3</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E6" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>45179.635998958329</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>8</v>
@@ -670,34 +2342,34 @@
       <c r="D7" s="4">
         <v>4</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>15</v>
+      <c r="E7" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>9</v>
       </c>
       <c r="G7" s="5"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>45179.636602615741</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E8" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>45179.637144444445</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>8</v>
@@ -705,20 +2377,20 @@
       <c r="D9" s="4">
         <v>4</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>13</v>
-      </c>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>45179.637515578703</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>8</v>
@@ -726,31 +2398,31 @@
       <c r="D10" s="4">
         <v>3</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>23</v>
+      <c r="E10" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>9</v>
       </c>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>45179.638177905093</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>45179.64942292824</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>8</v>
@@ -758,20 +2430,20 @@
       <c r="D12" s="4">
         <v>6</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>27</v>
+      <c r="E12" s="6" t="s">
+        <v>76</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G12" s="5"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>45179.649544444444</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>8</v>
@@ -779,20 +2451,20 @@
       <c r="D13" s="4">
         <v>6</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>27</v>
+      <c r="E13" s="6" t="s">
+        <v>76</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G13" s="5"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>45179.649611805551</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>8</v>
@@ -800,20 +2472,20 @@
       <c r="D14" s="4">
         <v>6</v>
       </c>
-      <c r="E14" s="4" t="s">
-        <v>27</v>
+      <c r="E14" s="6" t="s">
+        <v>76</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G14" s="5"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>45179.650675821758</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>8</v>
@@ -821,20 +2493,20 @@
       <c r="D15" s="4">
         <v>7</v>
       </c>
-      <c r="E15" s="4" t="s">
-        <v>23</v>
+      <c r="E15" s="6" t="s">
+        <v>64</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>9</v>
       </c>
       <c r="G15" s="5"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>45179.650714687501</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>8</v>
@@ -842,20 +2514,20 @@
       <c r="D16" s="4">
         <v>7</v>
       </c>
-      <c r="E16" s="4" t="s">
-        <v>23</v>
+      <c r="E16" s="6" t="s">
+        <v>65</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>9</v>
       </c>
       <c r="G16" s="5"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>45179.651202777779</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>8</v>
@@ -863,20 +2535,20 @@
       <c r="D17" s="4">
         <v>5</v>
       </c>
-      <c r="E17" s="4" t="s">
-        <v>31</v>
+      <c r="E17" s="6" t="s">
+        <v>77</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G17" s="5"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>45179.652719340273</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>8</v>
@@ -884,20 +2556,20 @@
       <c r="D18" s="4">
         <v>7</v>
       </c>
-      <c r="E18" s="4" t="s">
-        <v>23</v>
+      <c r="E18" s="6" t="s">
+        <v>66</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>9</v>
       </c>
       <c r="G18" s="5"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>45179.652771666668</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>8</v>
@@ -905,20 +2577,20 @@
       <c r="D19" s="4">
         <v>4</v>
       </c>
-      <c r="E19" s="4" t="s">
-        <v>34</v>
+      <c r="E19" s="6" t="s">
+        <v>78</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>9</v>
       </c>
       <c r="G19" s="5"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>45179.653060497687</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>8</v>
@@ -926,20 +2598,20 @@
       <c r="D20" s="4">
         <v>6</v>
       </c>
-      <c r="E20" s="4" t="s">
-        <v>36</v>
+      <c r="E20" s="6" t="s">
+        <v>67</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G20" s="5"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>45179.653443796298</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>8</v>
@@ -947,20 +2619,20 @@
       <c r="D21" s="4">
         <v>6</v>
       </c>
-      <c r="E21" s="4" t="s">
-        <v>38</v>
+      <c r="E21" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>9</v>
       </c>
       <c r="G21" s="5"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>45179.653703344906</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>8</v>
@@ -968,38 +2640,38 @@
       <c r="D22" s="4">
         <v>5</v>
       </c>
-      <c r="E22" s="4" t="s">
-        <v>36</v>
+      <c r="E22" s="6" t="s">
+        <v>67</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G22" s="5"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>45179.653890879628</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D23" s="4">
         <v>5</v>
       </c>
-      <c r="E23" s="4" t="s">
-        <v>41</v>
+      <c r="E23" s="6" t="s">
+        <v>72</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>9</v>
       </c>
       <c r="G23" s="5"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>45179.654957314815</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>8</v>
@@ -1007,16 +2679,16 @@
       <c r="D24" s="4">
         <v>8</v>
       </c>
-      <c r="E24" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E24" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>45179.655920335645</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>8</v>
@@ -1024,20 +2696,20 @@
       <c r="D25" s="4">
         <v>4</v>
       </c>
-      <c r="E25" s="4" t="s">
-        <v>41</v>
+      <c r="E25" s="6" t="s">
+        <v>72</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>9</v>
       </c>
       <c r="G25" s="5"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>45179.656328946759</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>8</v>
@@ -1045,20 +2717,20 @@
       <c r="D26" s="4">
         <v>5</v>
       </c>
-      <c r="E26" s="4" t="s">
-        <v>46</v>
+      <c r="E26" s="6" t="s">
+        <v>81</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G26" s="5"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>45179.656403090281</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>8</v>
@@ -1066,20 +2738,20 @@
       <c r="D27" s="4">
         <v>7</v>
       </c>
-      <c r="E27" s="4" t="s">
-        <v>48</v>
+      <c r="E27" s="6" t="s">
+        <v>82</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>9</v>
       </c>
       <c r="G27" s="5"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>45179.657247499999</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>8</v>
@@ -1087,31 +2759,31 @@
       <c r="D28" s="4">
         <v>5</v>
       </c>
-      <c r="E28" s="4" t="s">
-        <v>36</v>
+      <c r="E28" s="6" t="s">
+        <v>67</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G28" s="5"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>45179.657647280095</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>45179.658234953706</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>8</v>
@@ -1119,37 +2791,37 @@
       <c r="D30" s="4">
         <v>6</v>
       </c>
-      <c r="E30" s="4" t="s">
-        <v>48</v>
+      <c r="E30" s="6" t="s">
+        <v>83</v>
       </c>
       <c r="F30" s="4" t="s">
         <v>9</v>
       </c>
       <c r="G30" s="5"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>45179.658432268523</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="D31" s="4">
         <v>7</v>
       </c>
-      <c r="E31" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E31" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>45179.65850892361</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>8</v>
@@ -1157,37 +2829,37 @@
       <c r="D32" s="4">
         <v>5</v>
       </c>
-      <c r="E32" s="4" t="s">
-        <v>23</v>
+      <c r="E32" s="6" t="s">
+        <v>65</v>
       </c>
       <c r="F32" s="4" t="s">
         <v>9</v>
       </c>
       <c r="G32" s="5"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>45179.659201423608</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="D33" s="4">
         <v>6</v>
       </c>
-      <c r="E33" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E33" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>45179.659824432871</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>8</v>
@@ -1195,38 +2867,38 @@
       <c r="D34" s="4">
         <v>8</v>
       </c>
-      <c r="E34" s="4" t="s">
-        <v>38</v>
+      <c r="E34" s="6" t="s">
+        <v>84</v>
       </c>
       <c r="F34" s="4" t="s">
         <v>9</v>
       </c>
       <c r="G34" s="5"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>45179.660085717594</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="D35" s="4">
         <v>8</v>
       </c>
-      <c r="E35" s="4" t="s">
-        <v>59</v>
+      <c r="E35" s="6" t="s">
+        <v>85</v>
       </c>
       <c r="F35" s="4" t="s">
         <v>9</v>
       </c>
       <c r="G35" s="5"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>45179.660513935189</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>8</v>
@@ -1234,20 +2906,20 @@
       <c r="D36" s="4">
         <v>6</v>
       </c>
-      <c r="E36" s="4" t="s">
-        <v>23</v>
+      <c r="E36" s="6" t="s">
+        <v>65</v>
       </c>
       <c r="F36" s="4" t="s">
         <v>9</v>
       </c>
       <c r="G36" s="5"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>45179.66102049769</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>8</v>
@@ -1255,20 +2927,20 @@
       <c r="D37" s="4">
         <v>8</v>
       </c>
-      <c r="E37" s="4" t="s">
-        <v>61</v>
+      <c r="E37" s="6" t="s">
+        <v>86</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G37" s="5"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <v>45179.66148318287</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>8</v>
@@ -1276,62 +2948,62 @@
       <c r="D38" s="4">
         <v>5</v>
       </c>
-      <c r="E38" s="4" t="s">
-        <v>23</v>
+      <c r="E38" s="6" t="s">
+        <v>68</v>
       </c>
       <c r="F38" s="4" t="s">
         <v>9</v>
       </c>
       <c r="G38" s="5"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>45179.661542083333</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="D39" s="4">
         <v>8</v>
       </c>
-      <c r="E39" s="4" t="s">
-        <v>63</v>
+      <c r="E39" s="6" t="s">
+        <v>87</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G39" s="5"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
         <v>45179.661913749995</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="D40" s="4">
         <v>8</v>
       </c>
-      <c r="E40" s="4" t="s">
-        <v>65</v>
+      <c r="E40" s="6" t="s">
+        <v>88</v>
       </c>
       <c r="F40" s="4" t="s">
         <v>9</v>
       </c>
       <c r="G40" s="5"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <v>45179.66225572917</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>8</v>
@@ -1339,41 +3011,41 @@
       <c r="D41" s="4">
         <v>5</v>
       </c>
-      <c r="E41" s="4" t="s">
-        <v>59</v>
+      <c r="E41" s="6" t="s">
+        <v>89</v>
       </c>
       <c r="F41" s="4" t="s">
         <v>9</v>
       </c>
       <c r="G41" s="5"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
         <v>45179.662259652774</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="D42" s="4">
         <v>9</v>
       </c>
-      <c r="E42" s="4" t="s">
-        <v>67</v>
+      <c r="E42" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="F42" s="4" t="s">
         <v>9</v>
       </c>
       <c r="G42" s="5"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>45179.663080081024</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>8</v>
@@ -1381,7 +3053,7 @@
       <c r="D43" s="4">
         <v>5</v>
       </c>
-      <c r="E43" s="4" t="s">
+      <c r="E43" s="6" t="s">
         <v>69</v>
       </c>
       <c r="F43" s="4" t="s">
@@ -1389,29 +3061,29 @@
       </c>
       <c r="G43" s="5"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>45179.663509467588</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="D44" s="4">
         <v>2</v>
       </c>
-      <c r="E44" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E44" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>45179.664205138892</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>8</v>
@@ -1419,20 +3091,20 @@
       <c r="D45" s="4">
         <v>3</v>
       </c>
-      <c r="E45" s="4" t="s">
-        <v>41</v>
+      <c r="E45" s="6" t="s">
+        <v>74</v>
       </c>
       <c r="F45" s="4" t="s">
         <v>9</v>
       </c>
       <c r="G45" s="5"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <v>45179.665313344907</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>8</v>
@@ -1440,7 +3112,7 @@
       <c r="D46" s="4">
         <v>5</v>
       </c>
-      <c r="E46" s="4" t="s">
+      <c r="E46" s="6" t="s">
         <v>69</v>
       </c>
       <c r="F46" s="4" t="s">
@@ -1448,12 +3120,12 @@
       </c>
       <c r="G46" s="5"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>45179.666416539352</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>8</v>
@@ -1461,7 +3133,7 @@
       <c r="D47" s="4">
         <v>5</v>
       </c>
-      <c r="E47" s="4" t="s">
+      <c r="E47" s="6" t="s">
         <v>69</v>
       </c>
       <c r="F47" s="4" t="s">
@@ -1469,12 +3141,12 @@
       </c>
       <c r="G47" s="5"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
         <v>45179.666583530096</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>8</v>
@@ -1482,52 +3154,70 @@
       <c r="D48" s="4">
         <v>5</v>
       </c>
-      <c r="E48" s="4" t="s">
-        <v>69</v>
+      <c r="E48" s="6" t="s">
+        <v>70</v>
       </c>
       <c r="F48" s="4" t="s">
         <v>9</v>
       </c>
       <c r="G48" s="5"/>
     </row>
-    <row r="50" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C50" s="4" t="s">
-        <v>74</v>
+        <v>55</v>
       </c>
       <c r="D50" s="4">
         <f>AVERAGE(D2:D48)</f>
         <v>5.5909090909090908</v>
       </c>
     </row>
-    <row r="51" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C51" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="D51">
-        <f>SUM(D2:D48)</f>
-        <v>246</v>
-      </c>
-    </row>
-    <row r="52" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C52" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="D52">
-        <f>COUNT(D2:D48)</f>
-        <v>44</v>
-      </c>
-    </row>
-    <row r="53" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C53" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="D53">
-        <v>55.909090909090899</v>
+    <row r="59" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E59" t="s">
+        <v>56</v>
+      </c>
+      <c r="F59" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="60" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E60" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F60" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="61" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E61" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F61" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="62" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E62" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="63" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E63" s="7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="64" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E64" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="65" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E65" s="7" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup paperSize="9" fitToHeight="0" pageOrder="overThenDown" orientation="landscape" cellComments="atEnd"/>
+  <pageSetup paperSize="9" fitToHeight="0" pageOrder="overThenDown" orientation="landscape" cellComments="atEnd" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>